<commit_message>
Good version of 2nd lab
</commit_message>
<xml_diff>
--- a/laba_2/DB_2.xlsx
+++ b/laba_2/DB_2.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karbon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karbon\Desktop\database\laba_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72AC839-BFD7-4B7B-9951-94B2598F191B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B2BBC2-C451-4FF2-ADFC-1EFB65EA58F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="492" yWindow="5616" windowWidth="13884" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="additional_services" sheetId="1" r:id="rId1"/>
     <sheet name="additional_products" sheetId="4" r:id="rId2"/>
     <sheet name="clients" sheetId="2" r:id="rId3"/>
     <sheet name="additional_services_has_clients" sheetId="3" r:id="rId4"/>
-    <sheet name="additional_products_has_clients" sheetId="5" r:id="rId5"/>
+    <sheet name="client_has_additional_products" sheetId="5" r:id="rId5"/>
     <sheet name="warehouses" sheetId="9" r:id="rId6"/>
     <sheet name="additional_products_has_wh" sheetId="10" r:id="rId7"/>
     <sheet name="contracts" sheetId="6" r:id="rId8"/>
@@ -37,13 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>idadditional_services</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
   <si>
     <t>name</t>
   </si>
@@ -61,6 +55,186 @@
   </si>
   <si>
     <t>15 000</t>
+  </si>
+  <si>
+    <t>maker</t>
+  </si>
+  <si>
+    <t>Коврики для машины</t>
+  </si>
+  <si>
+    <t>Набор шин 16 диаметра</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Mazda</t>
+  </si>
+  <si>
+    <t>FIO</t>
+  </si>
+  <si>
+    <t>birthday</t>
+  </si>
+  <si>
+    <t>Быкадоров Михаил Юрьевич</t>
+  </si>
+  <si>
+    <t>Иванов Иван Иванович</t>
+  </si>
+  <si>
+    <t>10.01.2004</t>
+  </si>
+  <si>
+    <t>01.01.2000</t>
+  </si>
+  <si>
+    <t>adress</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>ул. Пушкина д. 31</t>
+  </si>
+  <si>
+    <t>ул. Пархоменко д. 15</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>10.04.2024</t>
+  </si>
+  <si>
+    <t>11.04.2024</t>
+  </si>
+  <si>
+    <t>Кузнецов Иван Петрович</t>
+  </si>
+  <si>
+    <t>Вишнева Инна Николаевна</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>Менеджер по продажам</t>
+  </si>
+  <si>
+    <t>Механик</t>
+  </si>
+  <si>
+    <t>60 000</t>
+  </si>
+  <si>
+    <t>50 000</t>
+  </si>
+  <si>
+    <t>id_additional_services_has_clients</t>
+  </si>
+  <si>
+    <t>id_additional_service</t>
+  </si>
+  <si>
+    <t>id_client</t>
+  </si>
+  <si>
+    <t>id_workers</t>
+  </si>
+  <si>
+    <t>id_additional_services</t>
+  </si>
+  <si>
+    <t>id_additional_product</t>
+  </si>
+  <si>
+    <t>id_client_has_additional_products</t>
+  </si>
+  <si>
+    <t>id_warehouses</t>
+  </si>
+  <si>
+    <t>free_space</t>
+  </si>
+  <si>
+    <t>id_additional_products_has_warehouses</t>
+  </si>
+  <si>
+    <t>id_additional_products</t>
+  </si>
+  <si>
+    <t>id_warehouse</t>
+  </si>
+  <si>
+    <t>id_contract</t>
+  </si>
+  <si>
+    <t>work_hours</t>
+  </si>
+  <si>
+    <t>id_position</t>
+  </si>
+  <si>
+    <t>id_car</t>
+  </si>
+  <si>
+    <t>colour</t>
+  </si>
+  <si>
+    <t>year_of_production</t>
+  </si>
+  <si>
+    <t>id_worker</t>
+  </si>
+  <si>
+    <t>id_model</t>
+  </si>
+  <si>
+    <t>id_provider</t>
+  </si>
+  <si>
+    <t>Черный</t>
+  </si>
+  <si>
+    <t>Белый</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>factory</t>
+  </si>
+  <si>
+    <t>Южная Корея</t>
+  </si>
+  <si>
+    <t>Китай</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Rio</t>
+  </si>
+  <si>
+    <t>Ceed</t>
+  </si>
+  <si>
+    <t>1 500 000</t>
+  </si>
+  <si>
+    <t>2 000 000</t>
   </si>
 </sst>
 </file>
@@ -381,47 +555,47 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -431,51 +605,50 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B880B898-592E-4F77-A28E-92C32F6BCBE9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B12BD8A-2AF8-415F-A0E3-D3FECD3F2017}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D2F225-F4B7-44F6-99CE-E5DD098FBA65}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE94CD67-8DD8-46B4-ADD6-38525E338A2F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -483,100 +656,680 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B12BD8A-2AF8-415F-A0E3-D3FECD3F2017}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2">
+        <v>2020</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3">
+        <v>2021</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D2F225-F4B7-44F6-99CE-E5DD098FBA65}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE94CD67-8DD8-46B4-ADD6-38525E338A2F}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA06B24F-1A02-4521-A640-9F2FF1470800}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="4" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>40000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DDC175-F828-443C-A735-FFE307278C27}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="31.21875" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B02BA0-0BE9-47CE-8CE8-D12118DF197F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2464AA4B-21EC-444F-9360-5A0D31F0E55E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCAAAD1-CE34-4BC6-B5A9-166F5C5E476A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="4" width="26.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1403D4-7BAE-4999-B3EC-BA699CF7C53C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75A21F4-2617-4522-96B0-AC066BCAC0CF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>575674624</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>878748343</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC9B667-FE00-4CC9-B8BA-E6AD0B925BEF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>112</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>63</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>